<commit_message>
updated model with graph
</commit_message>
<xml_diff>
--- a/inventory_management/input_data/seattle/item_sets.xlsx
+++ b/inventory_management/input_data/seattle/item_sets.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/chelseagreene/ws/github/epi_supplychain_optimization/inventory_management/input_data/seattle/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EFF286F5-FA8A-334F-96D5-86DEA2F4C4A3}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D979650A-61D1-AD45-82FE-069E86AD756A}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="100" yWindow="460" windowWidth="13400" windowHeight="16220" xr2:uid="{69866BB9-E712-2941-8958-B411B56F425F}"/>
+    <workbookView xWindow="13960" yWindow="560" windowWidth="13400" windowHeight="16220" xr2:uid="{69866BB9-E712-2941-8958-B411B56F425F}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="27">
   <si>
     <t>Item Type</t>
   </si>
@@ -103,6 +103,9 @@
   </si>
   <si>
     <t>Toilet Paper</t>
+  </si>
+  <si>
+    <t>Hand Santizer</t>
   </si>
 </sst>
 </file>
@@ -470,7 +473,7 @@
   <dimension ref="A1:F18"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D11" sqref="D11"/>
+      <selection activeCell="F13" sqref="F13:F18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -544,8 +547,23 @@
       </c>
     </row>
     <row r="4" spans="1:6">
+      <c r="A4">
+        <v>1</v>
+      </c>
+      <c r="B4" t="s">
+        <v>2</v>
+      </c>
+      <c r="C4">
+        <v>3</v>
+      </c>
       <c r="D4" s="1" t="s">
         <v>5</v>
+      </c>
+      <c r="E4">
+        <v>1</v>
+      </c>
+      <c r="F4">
+        <v>1</v>
       </c>
     </row>
     <row r="5" spans="1:6">
@@ -690,42 +708,152 @@
       </c>
     </row>
     <row r="12" spans="1:6">
+      <c r="A12">
+        <v>8</v>
+      </c>
+      <c r="B12" t="s">
+        <v>26</v>
+      </c>
+      <c r="C12">
+        <v>13</v>
+      </c>
       <c r="D12" s="3" t="s">
         <v>19</v>
       </c>
+      <c r="E12">
+        <v>8</v>
+      </c>
+      <c r="F12">
+        <v>3</v>
+      </c>
     </row>
     <row r="13" spans="1:6">
+      <c r="A13">
+        <v>8</v>
+      </c>
+      <c r="B13" t="s">
+        <v>26</v>
+      </c>
+      <c r="C13">
+        <v>14</v>
+      </c>
       <c r="D13" s="1" t="s">
         <v>20</v>
       </c>
+      <c r="E13">
+        <v>10</v>
+      </c>
+      <c r="F13">
+        <v>3</v>
+      </c>
     </row>
     <row r="14" spans="1:6">
+      <c r="A14">
+        <v>9</v>
+      </c>
+      <c r="B14" t="str">
+        <f>D14</f>
+        <v>Thermometers</v>
+      </c>
+      <c r="C14">
+        <v>15</v>
+      </c>
       <c r="D14" s="1" t="s">
         <v>21</v>
       </c>
+      <c r="E14">
+        <v>9</v>
+      </c>
+      <c r="F14">
+        <v>3</v>
+      </c>
     </row>
     <row r="15" spans="1:6">
+      <c r="A15">
+        <v>10</v>
+      </c>
+      <c r="B15" t="str">
+        <f t="shared" ref="B15:B18" si="0">D15</f>
+        <v>Isopropyl Alcohol (16oz bottle or equiv)</v>
+      </c>
+      <c r="C15">
+        <v>16</v>
+      </c>
       <c r="D15" s="1" t="s">
         <v>22</v>
       </c>
+      <c r="E15">
+        <v>10</v>
+      </c>
+      <c r="F15">
+        <v>3</v>
+      </c>
     </row>
     <row r="16" spans="1:6">
+      <c r="A16">
+        <v>11</v>
+      </c>
+      <c r="B16" t="str">
+        <f t="shared" si="0"/>
+        <v>Hand Soap</v>
+      </c>
+      <c r="C16">
+        <v>17</v>
+      </c>
       <c r="D16" s="1" t="s">
         <v>23</v>
       </c>
-    </row>
-    <row r="17" spans="4:4">
+      <c r="E16">
+        <v>10</v>
+      </c>
+      <c r="F16">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6">
+      <c r="A17">
+        <v>12</v>
+      </c>
+      <c r="B17" t="str">
+        <f t="shared" si="0"/>
+        <v>Facial Tissue</v>
+      </c>
+      <c r="C17">
+        <v>18</v>
+      </c>
       <c r="D17" s="1" t="s">
         <v>24</v>
       </c>
-    </row>
-    <row r="18" spans="4:4">
+      <c r="E17">
+        <v>10</v>
+      </c>
+      <c r="F17">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6">
+      <c r="A18">
+        <v>13</v>
+      </c>
+      <c r="B18" t="str">
+        <f t="shared" si="0"/>
+        <v>Toilet Paper</v>
+      </c>
+      <c r="C18">
+        <v>19</v>
+      </c>
       <c r="D18" s="1" t="s">
         <v>25</v>
       </c>
+      <c r="E18">
+        <v>10</v>
+      </c>
+      <c r="F18">
+        <v>3</v>
+      </c>
     </row>
   </sheetData>
-  <conditionalFormatting sqref="E2:E11">
+  <conditionalFormatting sqref="E2:E18">
     <cfRule type="colorScale" priority="11">
       <colorScale>
         <cfvo type="min"/>
@@ -745,7 +873,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="F2:F11">
+  <conditionalFormatting sqref="F2:F18">
     <cfRule type="colorScale" priority="15">
       <colorScale>
         <cfvo type="min"/>

</xml_diff>